<commit_message>
added more test case for excel read
</commit_message>
<xml_diff>
--- a/nodejs/excel/test_data.xlsx
+++ b/nodejs/excel/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\project\nodejs\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F371A15-1F6F-4ED5-BBCE-5A4BAE780E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BA9ED1-FE22-42C4-91BB-B23E6470119C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test-1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>S.No.</t>
   </si>
@@ -107,9 +107,6 @@
     <t>4_1</t>
   </si>
   <si>
-    <t>e1</t>
-  </si>
-  <si>
     <t>e2</t>
   </si>
   <si>
@@ -132,6 +129,27 @@
   </si>
   <si>
     <t>E2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>S_1</t>
+  </si>
+  <si>
+    <t>S_2</t>
+  </si>
+  <si>
+    <t>e6</t>
+  </si>
+  <si>
+    <t>e8</t>
+  </si>
+  <si>
+    <t>S_1_1</t>
   </si>
 </sst>
 </file>
@@ -537,7 +555,7 @@
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -916,19 +934,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{187DE655-AA37-44E9-B1C5-DA9AD2DB6309}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="12" max="12" width="13.26953125" customWidth="1"/>
-    <col min="13" max="13" width="12.54296875" customWidth="1"/>
+    <col min="13" max="13" width="13.26953125" customWidth="1"/>
+    <col min="14" max="14" width="12.54296875" customWidth="1"/>
+    <col min="15" max="15" width="12.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -939,16 +958,31 @@
         <v>24</v>
       </c>
       <c r="K1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
         <v>31</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>32</v>
       </c>
-      <c r="M1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -977,13 +1011,28 @@
         <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="M2" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+      <c r="N2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>